<commit_message>
[feat] add retry system
</commit_message>
<xml_diff>
--- a/backtest_results.xlsx
+++ b/backtest_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-07-17 16:32</t>
+          <t>2024-07-18 08:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,27 +492,27 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-07-17 16:33</t>
+          <t>2024-07-18 08:35</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -522,31 +522,31 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-07-17 16:34</t>
+          <t>2024-07-18 08:36</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -571,16 +571,16 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.89125</v>
+        <v>0.89</v>
       </c>
       <c r="H4" t="n">
-        <v>0.89125</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-07-17 16:35</t>
+          <t>2024-07-18 08:37</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -594,27 +594,27 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G5" t="n">
         <v>0.89</v>
       </c>
       <c r="H5" t="n">
-        <v>1.78125</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-07-17 16:36</t>
+          <t>2024-07-18 08:38</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -624,31 +624,31 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.89</v>
+        <v>0.892</v>
       </c>
       <c r="H6" t="n">
-        <v>1.78125</v>
+        <v>3.562</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-07-17 16:37</t>
+          <t>2024-07-18 08:39</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -662,10 +662,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -673,16 +673,16 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0.89</v>
+        <v>0.892</v>
       </c>
       <c r="H7" t="n">
-        <v>1.78125</v>
+        <v>3.562</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-07-17 16:38</t>
+          <t>2024-07-18 08:40</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -692,31 +692,31 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D8" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="E8" t="n">
         <v>2</v>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0.89125</v>
+        <v>0.892</v>
       </c>
       <c r="H8" t="n">
-        <v>2.6725</v>
+        <v>3.562</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-07-17 16:39</t>
+          <t>2024-07-18 08:41</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -730,27 +730,27 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>0.89125</v>
+        <v>0.8912</v>
       </c>
       <c r="H9" t="n">
-        <v>2.6725</v>
+        <v>4.4532</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-07-17 16:40</t>
+          <t>2024-07-18 08:42</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -760,14 +760,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -775,16 +775,16 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0.89125</v>
+        <v>0.8912</v>
       </c>
       <c r="H10" t="n">
-        <v>2.6725</v>
+        <v>4.4532</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-07-17 16:41</t>
+          <t>2024-07-18 08:43</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -794,14 +794,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>16</v>
+        <v>6.25</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0.89125</v>
+        <v>0.8912</v>
       </c>
       <c r="H11" t="n">
-        <v>2.6725</v>
+        <v>4.4532</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-07-17 16:42</t>
+          <t>2024-07-18 08:44</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -832,10 +832,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>32</v>
+        <v>15.625</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -843,16 +843,16 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0.89125</v>
+        <v>0.8912</v>
       </c>
       <c r="H12" t="n">
-        <v>2.6725</v>
+        <v>4.4532</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-07-17 16:43</t>
+          <t>2024-07-18 08:45</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -866,10 +866,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>64</v>
+        <v>39.0625</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -877,16 +877,16 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>0.89125</v>
+        <v>0.8912</v>
       </c>
       <c r="H13" t="n">
-        <v>2.6725</v>
+        <v>4.4532</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-07-17 16:45</t>
+          <t>2024-07-18 08:46</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -900,10 +900,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>128</v>
+        <v>97.65625</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>0.89125</v>
+        <v>0.8912</v>
       </c>
       <c r="H14" t="n">
-        <v>2.6725</v>
+        <v>4.4532</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024-07-17 16:46</t>
+          <t>2024-07-18 08:47</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -934,27 +934,27 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>244.140625</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0.8921875</v>
+        <v>0.8912</v>
       </c>
       <c r="H15" t="n">
-        <v>3.5646875</v>
+        <v>4.4532</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024-07-17 16:47</t>
+          <t>2024-07-18 08:48</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -979,16 +979,16 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0.89</v>
+        <v>0.89219072</v>
       </c>
       <c r="H16" t="n">
-        <v>4.454687499999999</v>
+        <v>5.34539072</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2024-07-17 16:48</t>
+          <t>2024-07-18 08:49</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -1013,16 +1013,16 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0.89</v>
+        <v>0.89219072</v>
       </c>
       <c r="H17" t="n">
-        <v>4.454687499999999</v>
+        <v>5.34539072</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2024-07-17 16:49</t>
+          <t>2024-07-18 08:50</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1032,11 +1032,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>8</v>
+        <v>6.25</v>
       </c>
       <c r="E18" t="n">
         <v>2</v>
@@ -1047,16 +1047,16 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0.89</v>
+        <v>0.89219072</v>
       </c>
       <c r="H18" t="n">
-        <v>4.454687499999999</v>
+        <v>5.34539072</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024-07-17 16:50</t>
+          <t>2024-07-18 08:51</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1066,31 +1066,31 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>15.625</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>0.89125</v>
+        <v>0.89219072</v>
       </c>
       <c r="H19" t="n">
-        <v>5.3459375</v>
+        <v>5.34539072</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2024-07-17 16:51</t>
+          <t>2024-07-18 08:52</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1104,27 +1104,27 @@
         </is>
       </c>
       <c r="D20" t="n">
+        <v>39.0625</v>
+      </c>
+      <c r="E20" t="n">
         <v>4</v>
       </c>
-      <c r="E20" t="n">
-        <v>1</v>
-      </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>LOSS</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>0.89125</v>
+        <v>0.89219072</v>
       </c>
       <c r="H20" t="n">
-        <v>5.3459375</v>
+        <v>5.34539072</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2024-07-17 16:52</t>
+          <t>2024-07-18 08:53</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1134,31 +1134,31 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>0.89125</v>
+        <v>0.8921600000000001</v>
       </c>
       <c r="H21" t="n">
-        <v>5.3459375</v>
+        <v>6.23755072</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2024-07-17 16:53</t>
+          <t>2024-07-18 08:54</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1168,14 +1168,14 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>16</v>
+        <v>2.5</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1183,16 +1183,16 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>0.89125</v>
+        <v>0.8921600000000001</v>
       </c>
       <c r="H22" t="n">
-        <v>5.3459375</v>
+        <v>6.23755072</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2024-07-17 16:54</t>
+          <t>2024-07-18 08:55</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1206,27 +1206,27 @@
         </is>
       </c>
       <c r="D23" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="E23" t="n">
         <v>2</v>
       </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0.891875</v>
+        <v>0.8921600000000001</v>
       </c>
       <c r="H23" t="n">
-        <v>6.2378125</v>
+        <v>6.23755072</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2024-07-17 16:55</t>
+          <t>2024-07-18 08:56</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1236,31 +1236,31 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2</v>
+        <v>15.625</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>0.89</v>
+        <v>0.8921600000000001</v>
       </c>
       <c r="H24" t="n">
-        <v>7.127812499999999</v>
+        <v>6.23755072</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2024-07-17 16:56</t>
+          <t>2024-07-18 08:57</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -1285,16 +1285,16 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>0.89</v>
+        <v>0.89216</v>
       </c>
       <c r="H25" t="n">
-        <v>8.0178125</v>
+        <v>7.129710719999999</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2024-07-17 16:57</t>
+          <t>2024-07-18 08:58</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1304,31 +1304,31 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G26" t="n">
         <v>0.89</v>
       </c>
       <c r="H26" t="n">
-        <v>8.0178125</v>
+        <v>8.019710719999999</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2024-07-17 16:58</t>
+          <t>2024-07-18 08:59</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1342,27 +1342,27 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G27" t="n">
         <v>0.89</v>
       </c>
       <c r="H27" t="n">
-        <v>8.0178125</v>
+        <v>8.90971072</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2024-07-17 16:59</t>
+          <t>2024-07-18 09:00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1372,14 +1372,14 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>16</v>
+        <v>2.5</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1390,13 +1390,13 @@
         <v>0.89</v>
       </c>
       <c r="H28" t="n">
-        <v>8.0178125</v>
+        <v>8.90971072</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2024-07-17 17:00</t>
+          <t>2024-07-18 09:01</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1410,7 +1410,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -1421,16 +1421,16 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>0.891875</v>
+        <v>0.892</v>
       </c>
       <c r="H29" t="n">
-        <v>8.9096875</v>
+        <v>9.801710719999999</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2024-07-17 17:01</t>
+          <t>2024-07-18 09:02</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1444,27 +1444,27 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>0.89</v>
+        <v>0.892</v>
       </c>
       <c r="H30" t="n">
-        <v>9.799687500000001</v>
+        <v>9.801710719999999</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2024-07-17 17:02</t>
+          <t>2024-07-18 09:03</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1474,14 +1474,14 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>4</v>
+        <v>6.25</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1489,16 +1489,16 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>0.89</v>
+        <v>0.892</v>
       </c>
       <c r="H31" t="n">
-        <v>9.799687500000001</v>
+        <v>9.801710719999999</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2024-07-17 17:03</t>
+          <t>2024-07-18 09:04</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1523,16 +1523,16 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>0.89</v>
+        <v>0.8912</v>
       </c>
       <c r="H32" t="n">
-        <v>10.6896875</v>
+        <v>10.69291072</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2024-07-17 17:04</t>
+          <t>2024-07-18 09:05</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1546,27 +1546,27 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G33" t="n">
         <v>0.89</v>
       </c>
       <c r="H33" t="n">
-        <v>10.6896875</v>
+        <v>11.58291072</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2024-07-17 17:05</t>
+          <t>2024-07-18 09:06</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1576,14 +1576,14 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1594,13 +1594,13 @@
         <v>0.89</v>
       </c>
       <c r="H34" t="n">
-        <v>10.6896875</v>
+        <v>11.58291072</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2024-07-17 17:06</t>
+          <t>2024-07-18 09:07</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1610,11 +1610,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -1625,16 +1625,16 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0.89125</v>
+        <v>0.892</v>
       </c>
       <c r="H35" t="n">
-        <v>11.5809375</v>
+        <v>12.47491072</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2024-07-17 17:07</t>
+          <t>2024-07-18 09:08</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1648,27 +1648,27 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0.89125</v>
+        <v>0.89</v>
       </c>
       <c r="H36" t="n">
-        <v>11.5809375</v>
+        <v>13.36491072</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2024-07-17 17:08</t>
+          <t>2024-07-18 09:09</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1678,31 +1678,31 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G37" t="n">
         <v>0.89</v>
       </c>
       <c r="H37" t="n">
-        <v>12.4709375</v>
+        <v>13.36491072</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2024-07-17 17:09</t>
+          <t>2024-07-18 09:10</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1716,27 +1716,27 @@
         </is>
       </c>
       <c r="D38" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="E38" t="n">
         <v>2</v>
       </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G38" t="n">
         <v>0.89</v>
       </c>
       <c r="H38" t="n">
-        <v>13.3609375</v>
+        <v>13.36491072</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2024-07-17 17:10</t>
+          <t>2024-07-18 09:11</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1746,31 +1746,31 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>15.625</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G39" t="n">
         <v>0.89</v>
       </c>
       <c r="H39" t="n">
-        <v>14.2509375</v>
+        <v>13.36491072</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2024-07-17 17:11</t>
+          <t>2024-07-18 09:12</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1780,31 +1780,31 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>0.89</v>
+        <v>0.89216</v>
       </c>
       <c r="H40" t="n">
-        <v>14.2509375</v>
+        <v>14.25707072</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2024-07-17 17:12</t>
+          <t>2024-07-18 09:13</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1818,7 +1818,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -1832,13 +1832,13 @@
         <v>0.89</v>
       </c>
       <c r="H41" t="n">
-        <v>15.1409375</v>
+        <v>15.14707072</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2024-07-17 17:13</t>
+          <t>2024-07-18 09:14</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="E42" t="n">
         <v>1</v>
@@ -1866,13 +1866,13 @@
         <v>0.89</v>
       </c>
       <c r="H42" t="n">
-        <v>15.1409375</v>
+        <v>15.14707072</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2024-07-17 17:15</t>
+          <t>2024-07-18 09:15</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1882,11 +1882,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUT </t>
+          <t>CALL</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>8</v>
+        <v>6.25</v>
       </c>
       <c r="E43" t="n">
         <v>2</v>
@@ -1900,13 +1900,13 @@
         <v>0.89</v>
       </c>
       <c r="H43" t="n">
-        <v>15.1409375</v>
+        <v>15.14707072</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2024-07-17 17:16</t>
+          <t>2024-07-18 09:16</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1916,11 +1916,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>16</v>
+        <v>15.625</v>
       </c>
       <c r="E44" t="n">
         <v>3</v>
@@ -1934,13 +1934,13 @@
         <v>0.89</v>
       </c>
       <c r="H44" t="n">
-        <v>15.1409375</v>
+        <v>15.14707072</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2024-07-17 17:17</t>
+          <t>2024-07-18 09:17</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1954,7 +1954,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>32</v>
+        <v>39.0625</v>
       </c>
       <c r="E45" t="n">
         <v>4</v>
@@ -1968,13 +1968,13 @@
         <v>0.89</v>
       </c>
       <c r="H45" t="n">
-        <v>15.1409375</v>
+        <v>15.14707072</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2024-07-17 17:18</t>
+          <t>2024-07-18 09:18</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1988,7 +1988,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>64</v>
+        <v>97.65625</v>
       </c>
       <c r="E46" t="n">
         <v>5</v>
@@ -2002,13 +2002,13 @@
         <v>0.89</v>
       </c>
       <c r="H46" t="n">
-        <v>15.1409375</v>
+        <v>15.14707072</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2024-07-17 17:19</t>
+          <t>2024-07-18 09:19</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -2033,16 +2033,16 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>0.8920312500000001</v>
+        <v>0.8921088</v>
       </c>
       <c r="H47" t="n">
-        <v>16.03296875</v>
+        <v>16.03917952</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2024-07-17 17:20</t>
+          <t>2024-07-18 09:20</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2056,27 +2056,27 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>0.8920312500000001</v>
+        <v>0.89</v>
       </c>
       <c r="H48" t="n">
-        <v>16.03296875</v>
+        <v>16.92917952</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2024-07-17 17:21</t>
+          <t>2024-07-18 09:21</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2086,31 +2086,31 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>WIN</t>
+          <t>LOSS</t>
         </is>
       </c>
       <c r="G49" t="n">
         <v>0.89</v>
       </c>
       <c r="H49" t="n">
-        <v>16.92296875</v>
+        <v>16.92917952</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2024-07-17 17:22</t>
+          <t>2024-07-18 09:22</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2120,31 +2120,31 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>CALL</t>
+          <t xml:space="preserve">PUT </t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>LOSS</t>
+          <t>WIN</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>0.89</v>
+        <v>0.892</v>
       </c>
       <c r="H50" t="n">
-        <v>16.92296875</v>
+        <v>17.82117952</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2024-07-17 17:23</t>
+          <t>2024-07-18 09:23</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2158,7 +2158,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -2172,7 +2172,347 @@
         <v>0.89</v>
       </c>
       <c r="H51" t="n">
-        <v>17.81296875</v>
+        <v>18.71117952</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-07-18 09:24</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUT </t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>WIN</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="H52" t="n">
+        <v>19.60117952</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-07-18 09:25</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUT </t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="H53" t="n">
+        <v>19.60117952</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-07-18 09:26</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>CALL</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>WIN</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>0.892</v>
+      </c>
+      <c r="H54" t="n">
+        <v>20.49317952</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-07-18 09:27</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>CALL</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>0.892</v>
+      </c>
+      <c r="H55" t="n">
+        <v>20.49317952</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-07-18 09:28</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUT </t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>0.892</v>
+      </c>
+      <c r="H56" t="n">
+        <v>20.49317952</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-07-18 09:29</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>CALL</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>WIN</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>0.8912</v>
+      </c>
+      <c r="H57" t="n">
+        <v>21.38437952</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-07-18 09:30</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>CALL</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>0.8912</v>
+      </c>
+      <c r="H58" t="n">
+        <v>21.38437952</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-07-18 09:32</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>CALL</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>0.8912</v>
+      </c>
+      <c r="H59" t="n">
+        <v>21.38437952</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-07-18 09:33</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUT </t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>WIN</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>0.8912</v>
+      </c>
+      <c r="H60" t="n">
+        <v>22.27557952</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-07-18 09:34</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUT </t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>0.8912</v>
+      </c>
+      <c r="H61" t="n">
+        <v>22.27557952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>